<commit_message>
Adjusted destination of some cases
</commit_message>
<xml_diff>
--- a/UseCaseActivityDEventTable/Event Table.xlsx
+++ b/UseCaseActivityDEventTable/Event Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaurapathirana/Documents/Academic/ACA 2020 - Third Sem (CS)/OOSD Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Software\XAMPP\htdocs\ArmyHospitalProject\UseCaseActivityDEventTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C93B92-859D-C346-ACDB-2BD338768D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4EFD94-73F8-4E74-9A02-B3FA29A91DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{3E76A909-DAB8-4740-A711-CC0DC9EAFB2A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3E76A909-DAB8-4740-A711-CC0DC9EAFB2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t xml:space="preserve">event </t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>admission officer wants to view patient profile</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>pateint record</t>
   </si>
 </sst>
 </file>
@@ -553,21 +559,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6C9B8C-0812-134B-AABB-571FE976F72A}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="215" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="58.83203125" customWidth="1"/>
+    <col min="1" max="1" width="53.296875" customWidth="1"/>
+    <col min="2" max="2" width="34.296875" customWidth="1"/>
+    <col min="3" max="3" width="16.296875" customWidth="1"/>
+    <col min="4" max="4" width="58.796875" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -607,7 +613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -627,7 +633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -647,7 +653,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -661,7 +667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -675,7 +681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -688,8 +694,14 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -702,8 +714,14 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -723,7 +741,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -736,8 +754,14 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -757,7 +781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -770,8 +794,11 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -791,7 +818,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -804,11 +831,14 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
       <c r="F14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -822,7 +852,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>

</xml_diff>